<commit_message>
Se corrigió la función de combinar materias
</commit_message>
<xml_diff>
--- a/Excel/Campeones.xlsx
+++ b/Excel/Campeones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Salvador\Documents\Generador de horarios\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7DE433-96FB-49FE-8D1E-483B48BDF7D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B77FF6-E0EE-46AF-9127-F1C6CD3198FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{F86EBB62-E59B-4753-B8AC-A23D1E40A9F6}"/>
+    <workbookView xWindow="16710" yWindow="4020" windowWidth="11415" windowHeight="11235" xr2:uid="{F86EBB62-E59B-4753-B8AC-A23D1E40A9F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -500,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -606,6 +606,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1046,7 +1049,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{49395621-77F4-4B39-B986-F8F12503B263}" name="Tabla1" displayName="Tabla1" ref="A1:J34" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9">
   <autoFilter ref="A1:J34" xr:uid="{49395621-77F4-4B39-B986-F8F12503B263}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I34">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J34">
     <sortCondition ref="A1:A34"/>
   </sortState>
   <tableColumns count="10">
@@ -1066,7 +1069,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1364,17 +1367,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393C4339-3F70-48E6-9D4D-F1C5E725DDDB}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1406,307 +1409,307 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="108.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>1645</v>
+        <v>840</v>
       </c>
       <c r="B2" s="1">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="I2" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J2" s="38"/>
     </row>
-    <row r="3" spans="1:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>1644</v>
-      </c>
-      <c r="B3" s="1">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1</v>
+    <row r="3" spans="1:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>1000</v>
+      </c>
+      <c r="B3" s="7">
+        <v>4</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0</v>
       </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="108.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>1644</v>
+        <v>1562</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="I4" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="B5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5" s="1">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>1644</v>
+      </c>
+      <c r="B6" s="1">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>6645</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="I6" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" ht="108.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>1562</v>
+        <v>1644</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="I7" s="1">
+        <v>2</v>
+      </c>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>1644</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="1">
         <v>0</v>
       </c>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>1645</v>
+      </c>
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="1">
+        <v>8</v>
+      </c>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>6562</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B10" s="1">
         <v>8</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="I8" s="1">
-        <v>5</v>
-      </c>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>6562</v>
-      </c>
-      <c r="B9" s="1">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I9" s="1">
-        <v>4</v>
-      </c>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>1643</v>
-      </c>
-      <c r="B10" s="1">
-        <v>4</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="I10" s="1">
         <v>5</v>
       </c>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="108.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>840</v>
+        <v>6562</v>
       </c>
       <c r="B11" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="I11" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>6644</v>
       </c>
@@ -1736,37 +1739,37 @@
       </c>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13">
-        <v>1000</v>
-      </c>
-      <c r="B13" s="7">
-        <v>4</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I13" s="3">
-        <v>0</v>
+    <row r="13" spans="1:10" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12">
+        <v>6645</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13" s="39">
+        <v>6</v>
       </c>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
       <c r="C14" s="34"/>
@@ -1778,7 +1781,7 @@
       <c r="I14" s="11"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
@@ -1790,7 +1793,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
@@ -1802,7 +1805,7 @@
       <c r="I16" s="3"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
@@ -1814,7 +1817,7 @@
       <c r="I17" s="3"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="27"/>
       <c r="B18" s="28"/>
       <c r="C18" s="29"/>
@@ -1826,7 +1829,7 @@
       <c r="I18" s="25"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
@@ -1838,7 +1841,7 @@
       <c r="I19" s="3"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="35"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
@@ -1850,7 +1853,7 @@
       <c r="I20" s="37"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
@@ -1862,7 +1865,7 @@
       <c r="I21" s="6"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
@@ -1874,7 +1877,7 @@
       <c r="I22" s="6"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13"/>
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
@@ -1886,7 +1889,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
@@ -1898,7 +1901,7 @@
       <c r="I24" s="3"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="9"/>
       <c r="C25" s="10"/>
@@ -1910,7 +1913,7 @@
       <c r="I25" s="3"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
@@ -1922,7 +1925,7 @@
       <c r="I26" s="6"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
@@ -1934,7 +1937,7 @@
       <c r="I27" s="3"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
@@ -1946,7 +1949,7 @@
       <c r="I28" s="3"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="8"/>
@@ -1958,7 +1961,7 @@
       <c r="I29" s="30"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="21"/>
       <c r="B30" s="18"/>
       <c r="C30" s="19"/>
@@ -1982,7 +1985,7 @@
       <c r="I31" s="6"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="21"/>
       <c r="B32" s="18"/>
       <c r="C32" s="19"/>
@@ -1994,7 +1997,7 @@
       <c r="I32" s="30"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="26"/>
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
@@ -2006,7 +2009,7 @@
       <c r="I33" s="30"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="31"/>
       <c r="B34" s="32"/>
       <c r="C34" s="33"/>
@@ -2028,7 +2031,7 @@
       <c r="G35" s="1"/>
       <c r="H35" s="11"/>
     </row>
-    <row r="36" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="12"/>
       <c r="B36" s="1"/>
       <c r="C36" s="2"/>
@@ -2056,7 +2059,7 @@
       <selection activeCell="I11" sqref="A10:I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A1" s="21">
@@ -2139,7 +2142,7 @@
       </c>
       <c r="I3" s="20"/>
     </row>
-    <row r="4" spans="1:9" ht="162.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="132" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1537</v>
       </c>

</xml_diff>

<commit_message>
Ya no trabaja paralelo pero es más rapido
</commit_message>
<xml_diff>
--- a/Excel/Campeones.xlsx
+++ b/Excel/Campeones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Salvador\Documents\Generador de horarios\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B77FF6-E0EE-46AF-9127-F1C6CD3198FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DD31F7-F7F0-4061-B090-9F3C0C33C370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16710" yWindow="4020" windowWidth="11415" windowHeight="11235" xr2:uid="{F86EBB62-E59B-4753-B8AC-A23D1E40A9F6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F86EBB62-E59B-4753-B8AC-A23D1E40A9F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="72">
   <si>
     <t>Clave</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>Nombre</t>
-  </si>
-  <si>
-    <t>Puntaje</t>
   </si>
   <si>
     <t>T</t>
@@ -261,6 +258,12 @@
   </si>
   <si>
     <t>English</t>
+  </si>
+  <si>
+    <t>9:00 a 11:00</t>
+  </si>
+  <si>
+    <t>Lun, Vie</t>
   </si>
 </sst>
 </file>
@@ -500,7 +503,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -593,9 +596,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -603,9 +603,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -615,47 +612,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <name val="Raleway"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FFDEE2E6"/>
-        </left>
-        <right style="medium">
-          <color rgb="FFDEE2E6"/>
-        </right>
-        <top style="medium">
-          <color rgb="FFDEE2E6"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FFDEE2E6"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <b val="0"/>
@@ -1047,22 +1004,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{49395621-77F4-4B39-B986-F8F12503B263}" name="Tabla1" displayName="Tabla1" ref="A1:J34" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9">
-  <autoFilter ref="A1:J34" xr:uid="{49395621-77F4-4B39-B986-F8F12503B263}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{49395621-77F4-4B39-B986-F8F12503B263}" name="Tabla1" displayName="Tabla1" ref="A1:I34" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
+  <autoFilter ref="A1:I34" xr:uid="{49395621-77F4-4B39-B986-F8F12503B263}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I34">
     <sortCondition ref="A1:A34"/>
   </sortState>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{7ED36AE9-82AC-43CA-A885-A6A446B149F9}" name="Clave" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{C348B707-798C-425E-8DC8-7287E925B3CD}" name="Gpo" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{91C40C7E-6072-4588-850D-FD15E445E1F6}" name="Profesor" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{7B52755E-F5A1-4235-8C10-D528C136A590}" name="Tipo" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{6D67F359-8F43-4333-AC7B-7202A51060C1}" name="Horario" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{44F0C552-7D0C-488F-8B21-12092FE36F1D}" name="Días" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{154482B2-8308-419E-BCB2-3E2DEDC13CF0}" name="Salón" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{2812DF78-91F2-447B-9C73-C051AA09F067}" name="Nombre" dataDxfId="1"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{7ED36AE9-82AC-43CA-A885-A6A446B149F9}" name="Clave" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{C348B707-798C-425E-8DC8-7287E925B3CD}" name="Gpo" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{91C40C7E-6072-4588-850D-FD15E445E1F6}" name="Profesor" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{7B52755E-F5A1-4235-8C10-D528C136A590}" name="Tipo" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{6D67F359-8F43-4333-AC7B-7202A51060C1}" name="Horario" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{44F0C552-7D0C-488F-8B21-12092FE36F1D}" name="Días" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{154482B2-8308-419E-BCB2-3E2DEDC13CF0}" name="Salón" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{2812DF78-91F2-447B-9C73-C051AA09F067}" name="Nombre" dataDxfId="0"/>
     <tableColumn id="9" xr3:uid="{E7E25FC3-F6A5-4F8B-AAB1-805C635C69B6}" name="Cupo"/>
-    <tableColumn id="10" xr3:uid="{8CC4DFB5-EB45-4156-8ABE-CB5E1E9F1654}" name="Puntaje" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1365,10 +1321,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393C4339-3F70-48E6-9D4D-F1C5E725DDDB}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,7 +1333,7 @@
     <col min="8" max="8" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1397,7 +1353,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H1" s="16" t="s">
         <v>7</v>
@@ -1405,11 +1361,8 @@
       <c r="I1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="108.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" ht="108.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>840</v>
       </c>
@@ -1417,29 +1370,28 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="I2" s="1">
         <v>3</v>
       </c>
-      <c r="J2" s="38"/>
-    </row>
-    <row r="3" spans="1:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1000</v>
       </c>
@@ -1447,29 +1399,28 @@
         <v>4</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>68</v>
-      </c>
       <c r="H3" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I3" s="7">
         <v>0</v>
       </c>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" ht="108.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9" ht="108.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1562</v>
       </c>
@@ -1477,29 +1428,28 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I4" s="1">
         <v>0</v>
       </c>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1643</v>
       </c>
@@ -1507,29 +1457,28 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="I5" s="1">
         <v>5</v>
       </c>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1644</v>
       </c>
@@ -1537,29 +1486,28 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I6" s="1">
         <v>1</v>
       </c>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:9" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1644</v>
       </c>
@@ -1567,29 +1515,28 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I7" s="1">
         <v>2</v>
       </c>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:9" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1644</v>
       </c>
@@ -1597,29 +1544,28 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I8" s="1">
         <v>0</v>
       </c>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1645</v>
       </c>
@@ -1627,29 +1573,28 @@
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="H9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I9" s="1">
         <v>8</v>
       </c>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:9" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>6562</v>
       </c>
@@ -1657,29 +1602,28 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="H10" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I10" s="1">
         <v>5</v>
       </c>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:9" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>6562</v>
       </c>
@@ -1687,29 +1631,28 @@
         <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="G11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I11" s="1">
         <v>4</v>
       </c>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:9" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>6644</v>
       </c>
@@ -1717,29 +1660,28 @@
         <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I12" s="1">
         <v>0</v>
       </c>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:9" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>6645</v>
       </c>
@@ -1747,41 +1689,57 @@
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H13" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="I13" s="39">
+      <c r="H13" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" s="37">
         <v>6</v>
       </c>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:9" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>1644</v>
+      </c>
+      <c r="B14" s="1">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
@@ -1791,9 +1749,8 @@
       <c r="G15" s="7"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
@@ -1803,9 +1760,8 @@
       <c r="G16" s="7"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
@@ -1815,9 +1771,8 @@
       <c r="G17" s="7"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="27"/>
       <c r="B18" s="28"/>
       <c r="C18" s="29"/>
@@ -1827,9 +1782,8 @@
       <c r="G18" s="28"/>
       <c r="H18" s="25"/>
       <c r="I18" s="25"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
@@ -1839,21 +1793,19 @@
       <c r="G19" s="7"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="34"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="36"/>
+    </row>
+    <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
@@ -1863,9 +1815,8 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="6"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
@@ -1875,9 +1826,8 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="6"/>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13"/>
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
@@ -1887,9 +1837,8 @@
       <c r="G23" s="7"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
@@ -1899,9 +1848,8 @@
       <c r="G24" s="7"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="9"/>
       <c r="C25" s="10"/>
@@ -1911,9 +1859,8 @@
       <c r="G25" s="9"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
@@ -1923,9 +1870,8 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="6"/>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
@@ -1935,9 +1881,8 @@
       <c r="G27" s="7"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
@@ -1947,9 +1892,8 @@
       <c r="G28" s="7"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
-      <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="8"/>
@@ -1959,9 +1903,8 @@
       <c r="G29" s="7"/>
       <c r="H29" s="4"/>
       <c r="I29" s="30"/>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="21"/>
       <c r="B30" s="18"/>
       <c r="C30" s="19"/>
@@ -1971,9 +1914,8 @@
       <c r="G30" s="18"/>
       <c r="H30" s="4"/>
       <c r="I30" s="6"/>
-      <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:9" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="32"/>
       <c r="B31" s="32"/>
       <c r="C31" s="33"/>
@@ -1983,9 +1925,8 @@
       <c r="G31" s="32"/>
       <c r="H31" s="4"/>
       <c r="I31" s="6"/>
-      <c r="J31" s="1"/>
-    </row>
-    <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="21"/>
       <c r="B32" s="18"/>
       <c r="C32" s="19"/>
@@ -1995,9 +1936,8 @@
       <c r="G32" s="18"/>
       <c r="H32" s="4"/>
       <c r="I32" s="30"/>
-      <c r="J32" s="1"/>
-    </row>
-    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="26"/>
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
@@ -2007,9 +1947,8 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="30"/>
-      <c r="J33" s="1"/>
-    </row>
-    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="31"/>
       <c r="B34" s="32"/>
       <c r="C34" s="33"/>
@@ -2019,9 +1958,8 @@
       <c r="G34" s="32"/>
       <c r="H34" s="11"/>
       <c r="I34" s="30"/>
-      <c r="J34" s="32"/>
-    </row>
-    <row r="35" spans="1:10" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:9" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="12"/>
       <c r="B35" s="1"/>
       <c r="C35" s="2"/>
@@ -2031,7 +1969,7 @@
       <c r="G35" s="1"/>
       <c r="H35" s="11"/>
     </row>
-    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="12"/>
       <c r="B36" s="1"/>
       <c r="C36" s="2"/>
@@ -2069,22 +2007,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="18" t="s">
         <v>9</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>10</v>
       </c>
       <c r="G1" s="18">
         <v>35</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I1" s="22"/>
     </row>
@@ -2096,22 +2034,22 @@
         <v>2</v>
       </c>
       <c r="C2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>35</v>
-      </c>
       <c r="F2" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G2" s="18">
         <v>35</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I2" s="23"/>
     </row>
@@ -2123,22 +2061,22 @@
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="1">
         <v>35</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I3" s="20"/>
     </row>
@@ -2150,22 +2088,22 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4" s="1">
         <v>35</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I4" s="24"/>
     </row>
@@ -2178,22 +2116,22 @@
         <v>2</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="F8" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>10</v>
       </c>
       <c r="G8" s="7">
         <v>35</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I8" s="3">
         <v>9.1999999999999993</v>

</xml_diff>